<commit_message>
fixed Fe uncertainties and reran scripts
</commit_message>
<xml_diff>
--- a/csdata/Fe/SI/Fe24+.xlsx
+++ b/csdata/Fe/SI/Fe24+.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmondeel/Documents/CfA/Chandra/CHANDRA-Rates/csdata/Fe/SI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73E3DD5-2B88-AC4A-ACA2-E5D1DA19E266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA349DAC-9B68-0B47-B115-316DA085A4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -137,6 +137,7 @@
     </xf>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,7 +359,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -434,7 +435,7 @@
       <c r="C3" s="5">
         <v>0.64</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -468,7 +469,7 @@
       <c r="C4" s="5">
         <v>0.92</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -502,7 +503,7 @@
       <c r="C5" s="5">
         <v>2.4</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -536,7 +537,7 @@
       <c r="C6" s="5">
         <v>4.8</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -560,7 +561,7 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -588,7 +589,7 @@
       <c r="Y7" s="4"/>
       <c r="Z7" s="4"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -616,7 +617,7 @@
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -644,7 +645,7 @@
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -672,7 +673,7 @@
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -700,7 +701,7 @@
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -728,7 +729,7 @@
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -756,7 +757,7 @@
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -784,7 +785,7 @@
       <c r="Y14" s="4"/>
       <c r="Z14" s="4"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -812,7 +813,7 @@
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -840,7 +841,7 @@
       <c r="Y16" s="4"/>
       <c r="Z16" s="4"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -868,7 +869,7 @@
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -896,7 +897,7 @@
       <c r="Y18" s="4"/>
       <c r="Z18" s="4"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -924,7 +925,7 @@
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -952,7 +953,7 @@
       <c r="Y20" s="4"/>
       <c r="Z20" s="4"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -980,7 +981,7 @@
       <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1008,7 +1009,7 @@
       <c r="Y22" s="4"/>
       <c r="Z22" s="4"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1036,7 +1037,7 @@
       <c r="Y23" s="4"/>
       <c r="Z23" s="4"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1064,7 +1065,7 @@
       <c r="Y24" s="4"/>
       <c r="Z24" s="4"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1092,7 +1093,7 @@
       <c r="Y25" s="4"/>
       <c r="Z25" s="4"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1120,7 +1121,7 @@
       <c r="Y26" s="4"/>
       <c r="Z26" s="4"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1148,7 +1149,7 @@
       <c r="Y27" s="4"/>
       <c r="Z27" s="4"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1176,7 +1177,7 @@
       <c r="Y28" s="4"/>
       <c r="Z28" s="4"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1204,7 +1205,7 @@
       <c r="Y29" s="4"/>
       <c r="Z29" s="4"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1230,7 +1231,7 @@
       <c r="Y30" s="4"/>
       <c r="Z30" s="4"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1256,7 +1257,7 @@
       <c r="Y31" s="4"/>
       <c r="Z31" s="4"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -1282,7 +1283,7 @@
       <c r="Y32" s="4"/>
       <c r="Z32" s="4"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -1308,7 +1309,7 @@
       <c r="Y33" s="4"/>
       <c r="Z33" s="4"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -1334,7 +1335,7 @@
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -1360,7 +1361,7 @@
       <c r="Y35" s="4"/>
       <c r="Z35" s="4"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -1386,7 +1387,7 @@
       <c r="Y36" s="4"/>
       <c r="Z36" s="4"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -1412,7 +1413,7 @@
       <c r="Y37" s="4"/>
       <c r="Z37" s="4"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -1438,7 +1439,7 @@
       <c r="Y38" s="4"/>
       <c r="Z38" s="4"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -1464,7 +1465,7 @@
       <c r="Y39" s="4"/>
       <c r="Z39" s="4"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -1490,7 +1491,7 @@
       <c r="Y40" s="4"/>
       <c r="Z40" s="4"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -1516,7 +1517,7 @@
       <c r="Y41" s="4"/>
       <c r="Z41" s="4"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -1542,7 +1543,7 @@
       <c r="Y42" s="4"/>
       <c r="Z42" s="4"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -1568,7 +1569,7 @@
       <c r="Y43" s="4"/>
       <c r="Z43" s="4"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -1594,7 +1595,7 @@
       <c r="Y44" s="4"/>
       <c r="Z44" s="4"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -1620,7 +1621,7 @@
       <c r="Y45" s="4"/>
       <c r="Z45" s="4"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -1646,7 +1647,7 @@
       <c r="Y46" s="4"/>
       <c r="Z46" s="4"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -1672,7 +1673,7 @@
       <c r="Y47" s="4"/>
       <c r="Z47" s="4"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -1698,7 +1699,7 @@
       <c r="Y48" s="4"/>
       <c r="Z48" s="4"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>

</xml_diff>